<commit_message>
Work from Monday 12/5/2016
</commit_message>
<xml_diff>
--- a/PerformanceTracker.xlsx
+++ b/PerformanceTracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>MARS</t>
+  </si>
+  <si>
+    <t>lm</t>
   </si>
 </sst>
 </file>
@@ -368,21 +371,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,7 +402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -413,10 +416,10 @@
         <v>9.2132290000000006E-2</v>
       </c>
       <c r="E2">
-        <v>3.6970459999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1061506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -430,10 +433,10 @@
         <v>8.9978719999999998E-2</v>
       </c>
       <c r="E3">
-        <v>6.0423299999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1116287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -447,10 +450,10 @@
         <v>6.0681069999999997E-2</v>
       </c>
       <c r="E4">
-        <v>6.303839E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.14699709999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -464,7 +467,63 @@
         <v>0.1106635</v>
       </c>
       <c r="E5">
-        <v>4.9366840000000002E-2</v>
+        <v>0.1053959</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>9.3469170000000004E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.12828000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>9.3826179999999995E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.1142764</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>5.3008699999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.13004679999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.1048269</v>
+      </c>
+      <c r="E9">
+        <v>0.1145216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work from 12/6/16
</commit_message>
<xml_diff>
--- a/PerformanceTracker.xlsx
+++ b/PerformanceTracker.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +538,44 @@
         <v>0.1145216</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0.1019815</v>
+      </c>
+      <c r="E10">
+        <v>0.1297403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>